<commit_message>
Update NWNDS Plains Master List.xlsx
</commit_message>
<xml_diff>
--- a/_notes_/Encounter Tables/NWNDS Plains Master List.xlsx
+++ b/_notes_/Encounter Tables/NWNDS Plains Master List.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3990" uniqueCount="1201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3991" uniqueCount="1201">
   <si>
     <t>Name</t>
   </si>
@@ -4306,10 +4306,10 @@
   <dimension ref="A1:AA1028"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B98" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B359" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C102" sqref="C102"/>
+      <selection pane="bottomRight" activeCell="G361" sqref="G361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1"/>
@@ -5069,8 +5069,8 @@
       <c r="K16" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="L16" s="43" t="s">
-        <v>71</v>
+      <c r="L16" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="M16" s="17" t="s">
         <v>18</v>
@@ -5111,8 +5111,8 @@
       <c r="K17" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="43" t="s">
-        <v>74</v>
+      <c r="L17" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="M17" s="17" t="s">
         <v>18</v>
@@ -5125,7 +5125,7 @@
       <c r="A18" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="2" t="s">
         <v>76</v>
       </c>
       <c r="C18" s="17" t="s">
@@ -5153,8 +5153,8 @@
       <c r="K18" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="L18" s="43" t="s">
-        <v>71</v>
+      <c r="L18" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="M18" s="17" t="s">
         <v>18</v>
@@ -7170,7 +7170,7 @@
       <c r="A61" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="2" t="s">
         <v>210</v>
       </c>
       <c r="C61" s="17" t="s">
@@ -7794,7 +7794,7 @@
       <c r="A75" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="B75" s="2" t="s">
         <v>245</v>
       </c>
       <c r="C75" s="17" t="s">
@@ -8466,7 +8466,7 @@
       <c r="A90" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="B90" s="17" t="s">
+      <c r="B90" s="2" t="s">
         <v>283</v>
       </c>
       <c r="C90" s="17" t="s">
@@ -9455,10 +9455,10 @@
       <c r="P110" s="17"/>
     </row>
     <row r="111" spans="1:27" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A111" s="17" t="s">
+      <c r="A111" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B111" s="17" t="s">
+      <c r="B111" s="2" t="s">
         <v>334</v>
       </c>
       <c r="C111" s="17" t="s">
@@ -9486,8 +9486,8 @@
       <c r="K111" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="L111" s="43">
-        <v>44564</v>
+      <c r="L111" s="43" t="s">
+        <v>138</v>
       </c>
       <c r="M111" s="17" t="s">
         <v>18</v>
@@ -11339,7 +11339,7 @@
       <c r="A151" s="17" t="s">
         <v>396</v>
       </c>
-      <c r="B151" s="17" t="s">
+      <c r="B151" s="2" t="s">
         <v>397</v>
       </c>
       <c r="C151" s="17" t="s">
@@ -12050,7 +12050,7 @@
       <c r="A167" s="17" t="s">
         <v>432</v>
       </c>
-      <c r="B167" s="17" t="s">
+      <c r="B167" s="2" t="s">
         <v>433</v>
       </c>
       <c r="C167" s="17" t="s">
@@ -12597,7 +12597,7 @@
       <c r="A179" s="17" t="s">
         <v>462</v>
       </c>
-      <c r="B179" s="17" t="s">
+      <c r="B179" s="2" t="s">
         <v>463</v>
       </c>
       <c r="C179" s="17" t="s">
@@ -13125,7 +13125,7 @@
       <c r="A191" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="B191" s="17" t="s">
+      <c r="B191" s="2" t="s">
         <v>490</v>
       </c>
       <c r="C191" s="17" t="s">
@@ -14758,7 +14758,7 @@
       <c r="A225" s="17" t="s">
         <v>562</v>
       </c>
-      <c r="B225" s="17" t="s">
+      <c r="B225" s="2" t="s">
         <v>563</v>
       </c>
       <c r="C225" s="17" t="s">
@@ -15496,7 +15496,7 @@
       <c r="A240" s="17" t="s">
         <v>600</v>
       </c>
-      <c r="B240" s="17" t="s">
+      <c r="B240" s="2" t="s">
         <v>601</v>
       </c>
       <c r="C240" s="17" t="s">
@@ -16123,7 +16123,7 @@
       <c r="A253" s="17" t="s">
         <v>630</v>
       </c>
-      <c r="B253" s="17" t="s">
+      <c r="B253" s="2" t="s">
         <v>631</v>
       </c>
       <c r="C253" s="17" t="s">
@@ -16176,7 +16176,7 @@
       <c r="A254" s="17" t="s">
         <v>632</v>
       </c>
-      <c r="B254" s="17" t="s">
+      <c r="B254" s="2" t="s">
         <v>633</v>
       </c>
       <c r="C254" s="17" t="s">
@@ -16271,7 +16271,7 @@
       <c r="A256" s="17" t="s">
         <v>636</v>
       </c>
-      <c r="B256" s="17" t="s">
+      <c r="B256" s="2" t="s">
         <v>637</v>
       </c>
       <c r="C256" s="17" t="s">
@@ -17109,7 +17109,7 @@
       <c r="A273" s="17" t="s">
         <v>674</v>
       </c>
-      <c r="B273" s="17" t="s">
+      <c r="B273" s="2" t="s">
         <v>675</v>
       </c>
       <c r="C273" s="17" t="s">
@@ -17679,7 +17679,7 @@
       <c r="A285" s="17" t="s">
         <v>700</v>
       </c>
-      <c r="B285" s="17" t="s">
+      <c r="B285" s="2" t="s">
         <v>701</v>
       </c>
       <c r="C285" s="17" t="s">
@@ -19506,7 +19506,7 @@
       <c r="A325" s="17" t="s">
         <v>780</v>
       </c>
-      <c r="B325" s="17" t="s">
+      <c r="B325" s="2" t="s">
         <v>781</v>
       </c>
       <c r="C325" s="17" t="s">
@@ -20154,7 +20154,7 @@
       <c r="A340" s="17" t="s">
         <v>814</v>
       </c>
-      <c r="B340" s="17" t="s">
+      <c r="B340" s="2" t="s">
         <v>815</v>
       </c>
       <c r="C340" s="17" t="s">
@@ -20454,10 +20454,10 @@
       <c r="AA345" s="3"/>
     </row>
     <row r="346" spans="1:27" ht="20.25" customHeight="1">
-      <c r="A346" s="17" t="s">
+      <c r="A346" s="2" t="s">
         <v>830</v>
       </c>
-      <c r="B346" s="17" t="s">
+      <c r="B346" s="2" t="s">
         <v>831</v>
       </c>
       <c r="C346" s="17" t="s">
@@ -20925,7 +20925,7 @@
       <c r="A356" s="17" t="s">
         <v>851</v>
       </c>
-      <c r="B356" s="17" t="s">
+      <c r="B356" s="2" t="s">
         <v>852</v>
       </c>
       <c r="C356" s="17" t="s">
@@ -21247,7 +21247,7 @@
       <c r="A363" s="17" t="s">
         <v>863</v>
       </c>
-      <c r="B363" s="17" t="s">
+      <c r="B363" s="2" t="s">
         <v>864</v>
       </c>
       <c r="C363" s="17" t="s">
@@ -21870,7 +21870,7 @@
       <c r="A375" s="17" t="s">
         <v>900</v>
       </c>
-      <c r="B375" s="17" t="s">
+      <c r="B375" s="2" t="s">
         <v>901</v>
       </c>
       <c r="C375" s="17" t="s">
@@ -24804,7 +24804,7 @@
       <c r="A429" s="17" t="s">
         <v>1011</v>
       </c>
-      <c r="B429" s="17" t="s">
+      <c r="B429" s="2" t="s">
         <v>1012</v>
       </c>
       <c r="C429" s="17" t="s">
@@ -26025,7 +26025,7 @@
       <c r="A452" s="47" t="s">
         <v>1052</v>
       </c>
-      <c r="B452" s="47" t="s">
+      <c r="B452" s="48" t="s">
         <v>1053</v>
       </c>
       <c r="C452" s="47" t="s">
@@ -27097,7 +27097,7 @@
       <c r="A472" s="47" t="s">
         <v>1096</v>
       </c>
-      <c r="B472" s="47" t="s">
+      <c r="B472" s="48" t="s">
         <v>1097</v>
       </c>
       <c r="C472" s="47" t="s">
@@ -27150,7 +27150,7 @@
       <c r="A473" s="47" t="s">
         <v>1098</v>
       </c>
-      <c r="B473" s="47" t="s">
+      <c r="B473" s="48" t="s">
         <v>1099</v>
       </c>
       <c r="C473" s="47" t="s">
@@ -28188,7 +28188,7 @@
       <autoFilter ref="A1:P443"/>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="L1:L8 L11:L37 L41:L50 L113:L117 L482:L1028 L222:L250 L255 L261:L353 L358:L360 Y358 L439:L442 L58:L111 L124:L143 L147:L152 L155:L212">
+  <conditionalFormatting sqref="L1:L8 L41:L50 L113:L117 L482:L1028 L222:L250 L255 L261:L353 L358:L360 Y358 L439:L442 L124:L143 L147:L152 L155:L212 L11:L37 L58:L111">
     <cfRule type="notContainsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(L1))&gt;0</formula>
     </cfRule>

</xml_diff>